<commit_message>
Scale back the COM32 adapter to only be used by the pyxll addin excelwrapper now only has read functions (IE. only used for compiling)
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -13,9 +13,10 @@
     <sheet name="trim-range" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="Missing">'trim-range'!#REF!</definedName>
     <definedName name="SINUS">Sheet1!$C$1:$C$18</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -663,7 +664,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
More test coverage and cleanup for excelcompiler
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15600" activeTab="3"/>
   </bookViews>
@@ -617,6 +617,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -634,6 +635,7 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -651,6 +653,7 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -661,10 +664,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -672,7 +675,7 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,8 +689,11 @@
       <c r="E1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -702,7 +708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="D3">
         <v>3</v>
       </c>
@@ -710,7 +716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="D4">
         <v>4</v>
       </c>
@@ -718,12 +724,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="D5">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
100% coverage for excelcompiler
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15600" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15600" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="trim-range" sheetId="4" r:id="rId4"/>
+    <sheet name="Empty" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Missing">'trim-range'!#REF!</definedName>
@@ -26,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>=SUM(D1:E3)</t>
   </si>
   <si>
     <t>=B1+SUM(D4:E4)+D5</t>
+  </si>
+  <si>
+    <t>=C1</t>
   </si>
 </sst>
 </file>
@@ -666,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -733,4 +737,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <f>C1</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Get table definitions from openpyxl
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -4,20 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15600" activeTab="4"/>
+    <workbookView xWindow="18255" yWindow="4395" windowWidth="25605" windowHeight="15825"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="trim-range" sheetId="4" r:id="rId4"/>
-    <sheet name="Empty" sheetId="5" r:id="rId5"/>
+    <sheet name="sref" sheetId="5" r:id="rId5"/>
+    <sheet name="Empty" sheetId="6" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="Missing">'trim-range'!#REF!</definedName>
+    <definedName name="Missing">'[1]trim-range'!#REF!</definedName>
     <definedName name="SINUS">Sheet1!$C$1:$C$18</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>=SUM(D1:E3)</t>
   </si>
@@ -35,7 +39,40 @@
     <t>=B1+SUM(D4:E4)+D5</t>
   </si>
   <si>
+    <t>col1</t>
+  </si>
+  <si>
+    <t>col2</t>
+  </si>
+  <si>
+    <t>col3</t>
+  </si>
+  <si>
+    <t>=SUM(Table1[col2])</t>
+  </si>
+  <si>
+    <t>=SUM(Table1)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>=C1</t>
+  </si>
+  <si>
+    <t>=SUM(Table1[#All])</t>
+  </si>
+  <si>
+    <t>=SUM(Table1[#Data])</t>
+  </si>
+  <si>
+    <t>=SUM(Table1[#Totals])</t>
+  </si>
+  <si>
+    <t>=SUM(Table1[#This Row])</t>
+  </si>
+  <si>
+    <t>=SUM(Table1[#Headers])</t>
   </si>
 </sst>
 </file>
@@ -71,16 +108,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="trim-range"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D1:F4" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="D1:F3"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="col1" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="col2" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="col3" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,9 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -621,7 +723,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -639,7 +741,7 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -655,9 +757,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -668,18 +774,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,11 +797,8 @@
       <c r="E1">
         <v>5</v>
       </c>
-      <c r="G1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -712,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:5">
       <c r="D3">
         <v>3</v>
       </c>
@@ -720,7 +821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:5">
       <c r="D4">
         <v>4</v>
       </c>
@@ -728,30 +829,150 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:5">
       <c r="D5">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <f>SUM(Table1[])</f>
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <f>SUM(Table1[col2])</f>
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <f>SUM(Table1[#This Row])</f>
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <f>SUM(Table1[#All])</f>
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <f>SUBTOTAL(109,[col3])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <f>SUM(Table1[#Data])</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[#Headers])</f>
+        <v>col1col2col3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <f>SUM(Table1[#Totals])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B1">
         <f>C1</f>
@@ -760,5 +981,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Workaround openpyxl converting numbers to datetimes
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18255" yWindow="4395" windowWidth="25605" windowHeight="15825"/>
+    <workbookView xWindow="18255" yWindow="4395" windowWidth="25605" windowHeight="15825" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,15 +13,16 @@
     <sheet name="trim-range" sheetId="4" r:id="rId4"/>
     <sheet name="sref" sheetId="5" r:id="rId5"/>
     <sheet name="Empty" sheetId="6" r:id="rId6"/>
+    <sheet name="datetime" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="Missing">'[1]trim-range'!#REF!</definedName>
     <definedName name="SINUS">Sheet1!$C$1:$C$18</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -108,12 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -983,4 +985,121 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>-2</v>
+      </c>
+      <c r="B1" s="3">
+        <f t="shared" ref="B1:B11" si="0">A1</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>58</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>59</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>60</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>61</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>62</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to openpyxl 2.6.0+
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -989,10 +989,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1005,7 +1005,7 @@
         <v>-2</v>
       </c>
       <c r="B1" s="3">
-        <f t="shared" ref="B1:B11" si="0">A1</f>
+        <f t="shared" ref="B1:B12" si="0">A1</f>
         <v>-2</v>
       </c>
     </row>
@@ -1097,6 +1097,15 @@
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>0.5</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement Array (CSE) formulas
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18255" yWindow="4395" windowWidth="25605" windowHeight="15825" activeTab="6"/>
+    <workbookView xWindow="18255" yWindow="4395" windowWidth="25605" windowHeight="15825" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,10 @@
     <sheet name="sref" sheetId="5" r:id="rId5"/>
     <sheet name="Empty" sheetId="6" r:id="rId6"/>
     <sheet name="datetime" sheetId="7" r:id="rId7"/>
+    <sheet name="ArrayForm" sheetId="8" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="Missing">'[1]trim-range'!#REF!</definedName>
@@ -80,13 +81,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,13 +115,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,7 +1003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1111,4 +1123,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4">
+        <f t="array" ref="C1">SUM(A1:A3*B1:B3)</f>
+        <v>71</v>
+      </c>
+      <c r="E1">
+        <f t="array" ref="E1:E3">ROW(A1:A3)</f>
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <f>INDEX(ROW(A1:A3), 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <f t="array" ref="H1:I1">COLUMN(A1:B1)</f>
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <f>INDEX(ROW(A1:A3), 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f>INDEX(COLUMN(A1:B1),1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>INDEX(COLUMN(A1:B1),1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="4">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <f>INDEX(ROW(A1:A3), 3)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement operators for Arrays
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>=SUM(D1:E3)</t>
   </si>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>=SUM(Table1[#Headers])</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1127,9 +1145,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -1200,6 +1220,136 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="array" ref="E7">SUM((A7:A13="a")*(B7:B13="y")*C7:C13)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="array" ref="E8">SUM((A7:A13&lt;&gt;"b")*(B7:B13&lt;&gt;"y")*C7:C13)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f t="array" ref="E9">SUM((A7:A13&gt;"b")*(B7:B13&lt;"z")*(C7:C13+3.5))</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <f t="array" ref="G16:H17">A16:B17*D16:E17</f>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add more info to Array Formulas index lookup
</commit_message>
<xml_diff>
--- a/tests/fixtures/excelcompiler.xlsx
+++ b/tests/fixtures/excelcompiler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18255" yWindow="4395" windowWidth="25605" windowHeight="15825" activeTab="7"/>
+    <workbookView xWindow="18255" yWindow="4395" windowWidth="25605" windowHeight="15825" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>=SUM(D1:E3)</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Expanding Array Formulas:</t>
   </si>
 </sst>
 </file>
@@ -152,19 +155,19 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -211,9 +214,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D1:F4" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="D1:F3"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="col1" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="2" name="col2" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="3" name="col3" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="col1" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="col2" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="3" name="col3" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -876,7 +879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -1145,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1330,7 +1335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1348,6 +1353,178 @@
       </c>
       <c r="H17">
         <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <f t="array" ref="E21:F24">A21:A24+C21:C24</f>
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <f t="array" ref="F28:I31">A21:A24*A30:D30</f>
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
+      <c r="H29">
+        <v>14</v>
+      </c>
+      <c r="I29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="F30">
+        <v>15</v>
+      </c>
+      <c r="G30">
+        <v>18</v>
+      </c>
+      <c r="H30">
+        <v>21</v>
+      </c>
+      <c r="I30">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="F31">
+        <v>20</v>
+      </c>
+      <c r="G31">
+        <v>24</v>
+      </c>
+      <c r="H31">
+        <v>28</v>
+      </c>
+      <c r="I31">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <f t="array" ref="A32:D33">A28:D28+A30:D30</f>
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>